<commit_message>
Finished LED Matrix Added part datasheets Updated BOM
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Anzahl</t>
   </si>
@@ -71,9 +71,6 @@
     <t>800167562 - VQ</t>
   </si>
   <si>
-    <t>D1 - D42</t>
-  </si>
-  <si>
     <t>TS2596SCS50</t>
   </si>
   <si>
@@ -87,6 +84,60 @@
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>40V 3A Schottky</t>
+  </si>
+  <si>
+    <t>B340A-13-F DII</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>FK 470/6,3 SP</t>
+  </si>
+  <si>
+    <t>470u</t>
+  </si>
+  <si>
+    <t>C3, C5</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>100p</t>
+  </si>
+  <si>
+    <t>C4, C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> µC</t>
+  </si>
+  <si>
+    <t>ESP32 WROOM 32D</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>1925467 - VQ</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>91R</t>
+  </si>
+  <si>
+    <t>RND 155HP05 EQ</t>
+  </si>
+  <si>
+    <t>KEM X7R0805 100N</t>
+  </si>
+  <si>
+    <t>100n</t>
   </si>
 </sst>
 </file>
@@ -419,15 +470,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -461,7 +512,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -480,6 +531,9 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
@@ -494,9 +548,6 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
@@ -506,16 +557,112 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LED-Matrix Baueilnummerierung hinzugefügt und BOM erweitert
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linda Heinrich\Siemens\2020\PSP20\hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6B1240-73A9-4617-A7DB-D13F29380534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-10020" yWindow="4335" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Anzahl</t>
   </si>
@@ -138,12 +139,21 @@
   </si>
   <si>
     <t>100n</t>
+  </si>
+  <si>
+    <t>D2, …, D43</t>
+  </si>
+  <si>
+    <t>R1, …, R42</t>
+  </si>
+  <si>
+    <t>C7, …, C48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,15 +203,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Anzahl"/>
-    <tableColumn id="2" name="Bauteil"/>
-    <tableColumn id="3" name="Wert"/>
-    <tableColumn id="5" name="Positionen"/>
-    <tableColumn id="6" name="Reichelt Best Nr."/>
-    <tableColumn id="4" name="Unrat Best Nr."/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wert"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positionen"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reichelt Best Nr."/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Unrat Best Nr."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -469,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +558,9 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
@@ -647,6 +660,9 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
       <c r="E10" t="s">
         <v>35</v>
       </c>
@@ -660,6 +676,9 @@
       </c>
       <c r="C11" t="s">
         <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Finished revision V1.0 Updated power supply input
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linda Heinrich\Siemens\2020\PSP20\hardware\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6B1240-73A9-4617-A7DB-D13F29380534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10020" yWindow="4335" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10020" yWindow="4335" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -105,9 +104,6 @@
     <t>C3, C5</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>100p</t>
   </si>
   <si>
@@ -148,12 +144,15 @@
   </si>
   <si>
     <t>C7, …, C48</t>
+  </si>
+  <si>
+    <t>D1, D44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,15 +202,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wert"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positionen"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reichelt Best Nr."/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Unrat Best Nr."/>
+    <tableColumn id="1" name="Anzahl"/>
+    <tableColumn id="2" name="Bauteil"/>
+    <tableColumn id="3" name="Wert"/>
+    <tableColumn id="5" name="Positionen"/>
+    <tableColumn id="6" name="Reichelt Best Nr."/>
+    <tableColumn id="4" name="Unrat Best Nr."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -479,11 +478,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -584,7 +583,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -593,7 +592,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -624,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -638,16 +637,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -655,16 +654,16 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -675,13 +674,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added LED matrix spaceing Added Soft-Reset Added Hard-Reset Added USB-Interface Added Programming-Button Added ISP-Programmer Created 3D Frontplate mockup
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>Anzahl</t>
   </si>
@@ -147,6 +147,69 @@
   </si>
   <si>
     <t>D1, D44</t>
+  </si>
+  <si>
+    <t>FT 232 RL</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>USB Type B</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>RND 205-00858</t>
+  </si>
+  <si>
+    <t>EVL 17-21SYGC/S2</t>
+  </si>
+  <si>
+    <t>LED Grün</t>
+  </si>
+  <si>
+    <t>LED Rot</t>
+  </si>
+  <si>
+    <t>D45</t>
+  </si>
+  <si>
+    <t>KBT KP-2012EC</t>
+  </si>
+  <si>
+    <t>R43, R44</t>
+  </si>
+  <si>
+    <t>RND 0805 1 220</t>
+  </si>
+  <si>
+    <t>D46</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>SMD Taster</t>
+  </si>
+  <si>
+    <t>SW1 - SW3</t>
+  </si>
+  <si>
+    <t>TASTER 1612.11</t>
   </si>
 </sst>
 </file>
@@ -479,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,6 +746,122 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>220</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>470</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Schematic to be more intuitive to read Updated BOM
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DL7MLP\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10641A32-8998-478C-9409-D72A33DE6828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10020" yWindow="4335" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-11505" yWindow="9495" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Anzahl</t>
   </si>
@@ -65,9 +66,6 @@
     <t>RGB</t>
   </si>
   <si>
-    <t>Unrat Best Nr.</t>
-  </si>
-  <si>
     <t>800167562 - VQ</t>
   </si>
   <si>
@@ -92,9 +90,6 @@
     <t>B340A-13-F DII</t>
   </si>
   <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
     <t>FK 470/6,3 SP</t>
   </si>
   <si>
@@ -143,9 +138,6 @@
     <t>R1, …, R42</t>
   </si>
   <si>
-    <t>C7, …, C48</t>
-  </si>
-  <si>
     <t>D1, D44</t>
   </si>
   <si>
@@ -197,9 +189,6 @@
     <t>D46</t>
   </si>
   <si>
-    <t>R45</t>
-  </si>
-  <si>
     <t>SW</t>
   </si>
   <si>
@@ -210,12 +199,42 @@
   </si>
   <si>
     <t>TASTER 1612.11</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>NPN Transistor</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>BCX 19 SMD</t>
+  </si>
+  <si>
+    <t>Conrad Best Nr.</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R45, R46, R47, R48</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>C7, …, C50</t>
+  </si>
+  <si>
+    <t>C1, C2, C51</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -249,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,15 +284,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:F19" totalsRowShown="0">
+  <autoFilter ref="A1:F19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Anzahl"/>
-    <tableColumn id="2" name="Bauteil"/>
-    <tableColumn id="3" name="Wert"/>
-    <tableColumn id="5" name="Positionen"/>
-    <tableColumn id="6" name="Reichelt Best Nr."/>
-    <tableColumn id="4" name="Unrat Best Nr."/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wert"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positionen"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reichelt Best Nr."/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Conrad Best Nr."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -541,14 +560,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
@@ -573,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -595,7 +614,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -604,7 +623,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -621,10 +640,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,16 +651,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,13 +671,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -669,13 +688,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,13 +705,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -700,16 +719,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -717,33 +736,33 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -751,16 +770,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,16 +787,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,13 +807,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -805,13 +824,13 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,35 +838,38 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16">
-        <v>220</v>
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17">
-        <v>470</v>
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
       </c>
       <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>58</v>
@@ -860,6 +882,20 @@
       </c>
       <c r="E18" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished PCB Layout V1 Updated Inductor for ripple reduction Rerouted FT232RL traces Added reset logic for ISP programming Added Silkscreen button labels
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DL7MLP\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10641A32-8998-478C-9409-D72A33DE6828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11505" yWindow="9495" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11505" yWindow="9495" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>Anzahl</t>
   </si>
@@ -229,12 +228,24 @@
   </si>
   <si>
     <t>C1, C2, C51</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>33uH</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L-PIHV4119 33µ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -284,15 +295,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:F19" totalsRowShown="0">
-  <autoFilter ref="A1:F19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F20" totalsRowShown="0">
+  <autoFilter ref="A1:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wert"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positionen"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reichelt Best Nr."/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Conrad Best Nr."/>
+    <tableColumn id="1" name="Anzahl"/>
+    <tableColumn id="2" name="Bauteil"/>
+    <tableColumn id="3" name="Wert"/>
+    <tableColumn id="5" name="Positionen"/>
+    <tableColumn id="6" name="Reichelt Best Nr."/>
+    <tableColumn id="4" name="Conrad Best Nr."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -560,14 +571,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
@@ -898,6 +909,23 @@
         <v>64</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished review of Layout Reviewed BOM Added input cutoff form screw terminal when barreljack is used Added branding Added revision Added author Optimised routing Added screw holes for case Updated barreljack footprint
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>Anzahl</t>
   </si>
@@ -182,9 +182,6 @@
     <t>R43, R44</t>
   </si>
   <si>
-    <t>RND 0805 1 220</t>
-  </si>
-  <si>
     <t>D46</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>R45, R46, R47, R48</t>
   </si>
   <si>
-    <t>220R</t>
-  </si>
-  <si>
     <t>C7, …, C50</t>
   </si>
   <si>
@@ -240,6 +234,30 @@
   </si>
   <si>
     <t>L-PIHV4119 33µ</t>
+  </si>
+  <si>
+    <t>Hohlbuchse</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>DC-BU 072759</t>
+  </si>
+  <si>
+    <t>300R</t>
+  </si>
+  <si>
+    <t>RND 0805 5 300</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Geprüft</t>
+  </si>
+  <si>
+    <t>RND 1550805 DN</t>
   </si>
 </sst>
 </file>
@@ -295,15 +313,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F20" totalsRowShown="0">
-  <autoFilter ref="A1:F20"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G21" totalsRowShown="0">
+  <autoFilter ref="A1:G21"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Anzahl"/>
     <tableColumn id="2" name="Bauteil"/>
     <tableColumn id="3" name="Wert"/>
     <tableColumn id="5" name="Positionen"/>
     <tableColumn id="6" name="Reichelt Best Nr."/>
     <tableColumn id="4" name="Conrad Best Nr."/>
+    <tableColumn id="7" name="Geprüft"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -572,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +605,7 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,10 +622,13 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -622,8 +644,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -634,13 +659,16 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>42</v>
       </c>
@@ -656,8 +684,11 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -673,8 +704,11 @@
       <c r="E5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -690,8 +724,11 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -707,8 +744,11 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -724,8 +764,11 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -741,8 +784,11 @@
       <c r="F9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>42</v>
       </c>
@@ -758,8 +804,11 @@
       <c r="E10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>44</v>
       </c>
@@ -770,13 +819,16 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -792,8 +844,11 @@
       <c r="E12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -804,13 +859,16 @@
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -826,8 +884,11 @@
       <c r="E14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -838,13 +899,16 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -852,78 +916,116 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
         <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>60</v>
       </c>
-      <c r="E18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
         <v>63</v>
       </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>69</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
         <v>70</v>
       </c>
-      <c r="E20" t="s">
-        <v>71</v>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated documentation Added datasheet for terminal block Updated BOM
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>Anzahl</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>RND 1550805 DN</t>
+  </si>
+  <si>
+    <t>Anschlussklemme</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>AKL 057-02</t>
   </si>
 </sst>
 </file>
@@ -313,8 +322,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G21" totalsRowShown="0">
-  <autoFilter ref="A1:G21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G22" totalsRowShown="0">
+  <autoFilter ref="A1:G22"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Anzahl"/>
     <tableColumn id="2" name="Bauteil"/>
@@ -591,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J30" sqref="I30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,6 +1037,23 @@
         <v>75</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added urgent features requested by client Added power LED Added option to supply complete PCB via USB port
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\Hardware\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DL7MLP\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72096085-9707-4FEB-B3B2-0100A82A0B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11505" yWindow="9495" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>Anzahl</t>
   </si>
@@ -173,15 +174,9 @@
     <t>LED Rot</t>
   </si>
   <si>
-    <t>D45</t>
-  </si>
-  <si>
     <t>KBT KP-2012EC</t>
   </si>
   <si>
-    <t>R43, R44</t>
-  </si>
-  <si>
     <t>D46</t>
   </si>
   <si>
@@ -267,12 +262,27 @@
   </si>
   <si>
     <t>AKL 057-02</t>
+  </si>
+  <si>
+    <t>D45, D47</t>
+  </si>
+  <si>
+    <t>R43, R44, R49</t>
+  </si>
+  <si>
+    <t>THT Schalter 2 Pol</t>
+  </si>
+  <si>
+    <t>SS ESP20</t>
+  </si>
+  <si>
+    <t>SW4, SW5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -306,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -322,16 +332,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G22" totalsRowShown="0">
-  <autoFilter ref="A1:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G23" totalsRowShown="0">
+  <autoFilter ref="A1:G23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Anzahl"/>
-    <tableColumn id="2" name="Bauteil"/>
-    <tableColumn id="3" name="Wert"/>
-    <tableColumn id="5" name="Positionen"/>
-    <tableColumn id="6" name="Reichelt Best Nr."/>
-    <tableColumn id="4" name="Conrad Best Nr."/>
-    <tableColumn id="7" name="Geprüft"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wert"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positionen"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reichelt Best Nr."/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Conrad Best Nr."/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Geprüft"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,14 +609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="I30:J30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
@@ -631,10 +641,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -654,7 +664,7 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,13 +678,13 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -694,7 +704,7 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,7 +724,7 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,7 +744,7 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -754,7 +764,7 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -774,7 +784,7 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -794,7 +804,7 @@
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -814,7 +824,7 @@
         <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -828,13 +838,13 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -854,7 +864,7 @@
         <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,18 +878,18 @@
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -888,13 +898,13 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
         <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -908,33 +918,33 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -942,19 +952,19 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>56</v>
-      </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -962,19 +972,19 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -985,16 +995,16 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1002,19 +1012,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
         <v>66</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1025,16 +1035,16 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,13 +1055,36 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" t="s">
-        <v>80</v>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Layout V1 Created Gerber and Excellion drill files Updated BOM Added order manual Added orderlist Updated Schematic
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DL7MLP\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72096085-9707-4FEB-B3B2-0100A82A0B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92313C86-F002-40C1-A62C-8F3E511C8CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15675" yWindow="-120" windowWidth="13500" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>Anzahl</t>
   </si>
@@ -210,9 +219,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>R45, R46, R47, R48</t>
-  </si>
-  <si>
     <t>C7, …, C50</t>
   </si>
   <si>
@@ -276,7 +282,28 @@
     <t>SS ESP20</t>
   </si>
   <si>
-    <t>SW4, SW5</t>
+    <t>OP07</t>
+  </si>
+  <si>
+    <t>OP 07 CD</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>P-FET</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>NDS 0610 SMD</t>
+  </si>
+  <si>
+    <t>R45 - R48, R50, R51</t>
+  </si>
+  <si>
+    <t>SW4</t>
   </si>
 </sst>
 </file>
@@ -332,8 +359,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G23" totalsRowShown="0">
-  <autoFilter ref="A1:G23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G25" totalsRowShown="0">
+  <autoFilter ref="A1:G25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
@@ -610,16 +637,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -644,7 +671,7 @@
         <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -664,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -678,53 +705,53 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,19 +759,19 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -755,116 +782,116 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -872,139 +899,139 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
         <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1012,19 +1039,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1032,19 +1059,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1052,39 +1079,79 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM to match PCB Rev V1.1
</commit_message>
<xml_diff>
--- a/Dokumentation/BOM.xlsx
+++ b/Dokumentation/BOM.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DL7MLP\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Sees\PSP20\Hardware\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92313C86-F002-40C1-A62C-8F3E511C8CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15675" yWindow="-120" windowWidth="13500" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15675" yWindow="-120" windowWidth="13500" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
   <si>
     <t>Anzahl</t>
   </si>
@@ -105,9 +104,6 @@
     <t>470u</t>
   </si>
   <si>
-    <t>C3, C5</t>
-  </si>
-  <si>
     <t>100p</t>
   </si>
   <si>
@@ -300,16 +296,34 @@
     <t>NDS 0610 SMD</t>
   </si>
   <si>
-    <t>R45 - R48, R50, R51</t>
-  </si>
-  <si>
     <t>SW4</t>
+  </si>
+  <si>
+    <t>Legacy</t>
+  </si>
+  <si>
+    <t>DMP 3098L7 DII</t>
+  </si>
+  <si>
+    <t>KEM C0G0805 100P</t>
+  </si>
+  <si>
+    <t>R45 - R48, R50 - R52</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>ECC MZS350ARA471</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,16 +373,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:G25" totalsRowShown="0">
-  <autoFilter ref="A1:G25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Anzahl"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bauteil"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Wert"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positionen"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reichelt Best Nr."/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Conrad Best Nr."/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Geprüft"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H26" totalsRowShown="0">
+  <autoFilter ref="A1:H26"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Anzahl"/>
+    <tableColumn id="2" name="Bauteil"/>
+    <tableColumn id="3" name="Wert"/>
+    <tableColumn id="5" name="Positionen"/>
+    <tableColumn id="6" name="Reichelt Best Nr."/>
+    <tableColumn id="4" name="Conrad Best Nr."/>
+    <tableColumn id="7" name="Geprüft"/>
+    <tableColumn id="8" name="Legacy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,22 +651,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,13 +684,16 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -691,10 +710,10 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -705,16 +724,16 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -731,10 +750,10 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -745,18 +764,18 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -765,393 +784,419 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="G8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
       <c r="G14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="G15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E17" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>74</v>
       </c>
-      <c r="G17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24">
+        <v>60</v>
+      </c>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
         <v>13</v>
       </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
         <v>27</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F26" t="s">
         <v>28</v>
       </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" t="s">
-        <v>72</v>
+      <c r="G26" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>